<commit_message>
CUS15: ajustes en controlador y cotizaciones
</commit_message>
<xml_diff>
--- a/src/Cotizaciones/REC2000_20123456789.xlsx
+++ b/src/Cotizaciones/REC2000_20123456789.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mundo-patitas\src\Cotizaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C0DB2-BC2E-4A45-9EDA-11A10D2584C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B65178-77E4-4EEB-AB06-8D84BE79F29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1128" yWindow="3144" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COTIZACION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Datos del Cliente</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>NOTA: El sistema leerá solo los campos necesarios. El Id_Requerimiento se tomará del nombre de archivo REC{IdReq}_{RUC}.xlsx</t>
   </si>
   <si>
     <t>hugovertiz71@gmail.com</t>
@@ -262,7 +259,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -296,11 +293,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -692,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,10 +703,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -720,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -754,7 +752,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -796,7 +794,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>18</v>
@@ -827,7 +825,7 @@
         <v>1046</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="4">
         <v>50</v>
@@ -845,7 +843,7 @@
         <v>1027</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="4">
         <v>30</v>
@@ -863,7 +861,7 @@
         <v>1026</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4">
         <v>100</v>
@@ -904,13 +902,11 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="11"/>
@@ -921,9 +917,8 @@
       <c r="D31" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A25:E25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{9AFCD020-A123-4151-A138-EB51AD32A02B}"/>

</xml_diff>

<commit_message>
CUS15: actualización de servicios, scripts y archivos de cotización
</commit_message>
<xml_diff>
--- a/src/Cotizaciones/REC2000_20123456789.xlsx
+++ b/src/Cotizaciones/REC2000_20123456789.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mundo-patitas\src\Cotizaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B65178-77E4-4EEB-AB06-8D84BE79F29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C617D15-EA1F-4306-97C8-52CAD6DC1798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1392" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COTIZACION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Datos del Cliente</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Cotización de Productos</t>
+  </si>
+  <si>
+    <t>Cotizacion N°</t>
   </si>
 </sst>
 </file>
@@ -296,9 +299,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -690,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,10 +706,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1">
+        <v>600231</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -903,10 +912,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="11"/>

</xml_diff>

<commit_message>
Actualización de CUS15: mejoras en OrdenCompra, PDF y archivos Excel
</commit_message>
<xml_diff>
--- a/src/Cotizaciones/REC2000_20123456789.xlsx
+++ b/src/Cotizaciones/REC2000_20123456789.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mundo-patitas\src\Cotizaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C617D15-EA1F-4306-97C8-52CAD6DC1798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC197D7-E11B-4F8A-A97D-FC78E98E322E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1392" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1992" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COTIZACION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Datos del Cliente</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Contacto:</t>
   </si>
   <si>
-    <t>Nombre y teléfono</t>
-  </si>
-  <si>
     <t>Datos del Emisor (Proveedor)</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>FechaRecepcion (opcional)</t>
   </si>
   <si>
-    <t>Av. Ejemplo 123, Lima</t>
-  </si>
-  <si>
     <t>Moneda</t>
   </si>
   <si>
@@ -139,6 +133,24 @@
   </si>
   <si>
     <t>Cotizacion N°</t>
+  </si>
+  <si>
+    <t>Filtro para Acuario 3L</t>
+  </si>
+  <si>
+    <t>Snack Mixto Para Aves Tropicales 500g</t>
+  </si>
+  <si>
+    <t>Snack Saludable Para Perro 100g</t>
+  </si>
+  <si>
+    <t>Suéter para Perro Mediano</t>
+  </si>
+  <si>
+    <t>Cepillo Dental Para Perro Medium</t>
+  </si>
+  <si>
+    <t>Av. Ejemplo 123, Los Olivos</t>
   </si>
 </sst>
 </file>
@@ -215,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -254,6 +266,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -262,7 +283,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -300,6 +321,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -331,7 +355,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FFD9D9D9"/>
         </left>
@@ -344,6 +368,8 @@
         <bottom style="thin">
           <color rgb="FFD9D9D9"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -364,7 +390,7 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FFD9D9D9"/>
         </left>
@@ -377,6 +403,8 @@
         <bottom style="thin">
           <color rgb="FFD9D9D9"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -393,8 +421,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Detalle" displayName="Detalle" ref="A16:E19">
-  <autoFilter ref="A16:E19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Detalle" displayName="Detalle" ref="A16:E24">
+  <autoFilter ref="A16:E24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:E23">
+    <sortCondition ref="B16:B23"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id_Producto" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripcion" dataDxfId="1"/>
@@ -691,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,15 +737,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="18"/>
+      <c r="A1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="21"/>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1">
-        <v>600231</v>
+        <v>60023</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -727,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -750,38 +781,38 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7">
+        <v>987654321</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" t="s">
         <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -789,70 +820,70 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
         <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
-        <v>1046</v>
+        <v>1019</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C17" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4">
         <v>10</v>
       </c>
       <c r="E17" s="5">
-        <f>IFERROR(C17*D17,"")</f>
-        <v>500</v>
+        <f t="shared" ref="E17:E24" si="0">IFERROR(C17*D17,"")</f>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
-        <v>1027</v>
+        <v>1045</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4">
         <v>30</v>
@@ -861,69 +892,160 @@
         <v>8</v>
       </c>
       <c r="E18" s="5">
-        <f>IFERROR(C18*D18,"")</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
+        <v>1029</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="4">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>1036</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="4">
+        <v>20</v>
+      </c>
+      <c r="D20" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>1047</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
+        <v>1046</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4">
+        <v>30</v>
+      </c>
+      <c r="D22" s="4">
+        <v>8</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
         <v>1026</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="4">
         <v>100</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D23" s="4">
         <v>5</v>
       </c>
-      <c r="E19" s="5">
-        <f>IFERROR(C19*D19,"")</f>
+      <c r="E23" s="5">
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D21" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="12">
+        <v>1027</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="19">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>6.5</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="6">
+        <f>SUM(E17:E24)</f>
+        <v>1827.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="6">
+        <f>ROUND(E26*0.18,2)</f>
+        <v>328.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="6">
-        <f>SUM(E17:E19)</f>
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="6">
-        <f>ROUND(E21*0.18,2)</f>
-        <v>223.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="7">
-        <f>E21+E22</f>
-        <v>1463.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="11"/>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="11"/>
-      <c r="D31" s="10"/>
+      <c r="E28" s="7">
+        <f>E26+E27</f>
+        <v>2156.4499999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+    </row>
+    <row r="35" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="11"/>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="11"/>
+      <c r="D36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>